<commit_message>
Updated labeling for health-table 8, 10 and 11
</commit_message>
<xml_diff>
--- a/sources/fact_extraction_viewpoint/health-table08.xlsx
+++ b/sources/fact_extraction_viewpoint/health-table08.xlsx
@@ -113,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -197,7 +197,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -206,18 +206,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,10 +226,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,8 +252,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -789,7 +786,7 @@
   <dimension ref="B1:Q165"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="N6" sqref="N6:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -817,7 +814,7 @@
       <c r="N3" s="4"/>
     </row>
     <row r="4" spans="2:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="F4" s="4"/>
@@ -848,61 +845,61 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="29" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="21" t="s">
         <v>1</v>
       </c>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="2:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="I7" s="24"/>
-      <c r="J7" s="26" t="s">
+      <c r="I7" s="23"/>
+      <c r="J7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="26" t="s">
+      <c r="K7" s="23"/>
+      <c r="L7" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="22" t="s">
+      <c r="M7" s="23"/>
+      <c r="N7" s="21" t="s">
         <v>4</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="2:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="23" t="s">
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="22" t="s">
         <v>5</v>
       </c>
       <c r="Q8" s="1"/>
@@ -1088,7 +1085,7 @@
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="2:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>13</v>
       </c>
       <c r="J19" s="4"/>
@@ -1096,7 +1093,7 @@
       <c r="Q19" s="1"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="10"/>
@@ -1108,12 +1105,12 @@
       <c r="Q20" s="1"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="13" x14ac:dyDescent="0.3">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1133,51 +1130,51 @@
       <c r="Q24" s="1"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
       <c r="Q25" s="1"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
       <c r="Q26" s="1"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">

</xml_diff>